<commit_message>
added POM for Login page and added test method for verification of homepage title(for login test with valid credentials)
</commit_message>
<xml_diff>
--- a/excelTestCaseDoc/nopCommerce.xlsx
+++ b/excelTestCaseDoc/nopCommerce.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\nopCommerceProject\excelTestCaseDoc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{132643A1-F507-426B-91AC-EA4AB8F77E7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD1579BF-7A23-42E2-9FA7-55F80E9F1019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>Title</t>
   </si>
@@ -65,15 +65,43 @@
     <t>Actual Title should match with expected</t>
   </si>
   <si>
-    <t>Actual Title:
+    <t>check login</t>
+  </si>
+  <si>
+    <t>while enterig valid username and password it should navigate us to the homepage</t>
+  </si>
+  <si>
+    <t>1.hit the url
+2.enter valid username
+3.enter valid password
+4.click login button</t>
+  </si>
+  <si>
+    <t>Expected Title of Login Page:
 "Your store. Login"</t>
+  </si>
+  <si>
+    <t>As Expected</t>
+  </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>1. Login Page and Home page title verification</t>
+  </si>
+  <si>
+    <t>usename:admin@
+yourstore.com
+password:admin
+Expected Title of Login Page:
+"Dashboard / nopCommerce administration"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -81,8 +109,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="14"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="14"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -92,6 +152,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -123,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -131,22 +203,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -154,10 +213,37 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -165,6 +251,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFF00"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -439,193 +530,222 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="30.7109375" style="10" customWidth="1"/>
-    <col min="3" max="3" width="40.7109375" style="9" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15" style="10" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" style="10" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="40.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" style="9" customWidth="1"/>
+    <col min="5" max="5" width="24" style="5" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" style="5" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" customWidth="1"/>
     <col min="8" max="8" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="10" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="12">
-        <v>1</v>
-      </c>
-      <c r="B2" s="12" t="s">
+    <row r="2" spans="1:8" s="12" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+    </row>
+    <row r="3" spans="1:8" s="5" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>101</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D3" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E3" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="120" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>101</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="C4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="12"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="12"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>4</v>
-      </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
+      <c r="A5" s="3">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
-        <v>5</v>
-      </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
+      <c r="A6" s="3">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
-        <v>6</v>
-      </c>
-      <c r="B7" s="12"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
+      <c r="A7" s="3">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
-        <v>7</v>
-      </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
+      <c r="A8" s="3">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
       <c r="G8" s="3"/>
       <c r="H8" s="3"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
-        <v>8</v>
-      </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
+      <c r="A9" s="3">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
-        <v>9</v>
-      </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
+      <c r="A10" s="3">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
-        <v>10</v>
-      </c>
-      <c r="B11" s="12"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="7"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
+      <c r="A11" s="3">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
-        <v>11</v>
-      </c>
-      <c r="B12" s="12"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
+      <c r="A12" s="3">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
     </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:H2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>